<commit_message>
fix(#106): loan template disallow user to select column headers
</commit_message>
<xml_diff>
--- a/AccuPay.Web/ImportTemplates/accupay-loan-template.xlsx
+++ b/AccuPay.Web/ImportTemplates/accupay-loan-template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="19890" windowHeight="8355" tabRatio="500" activeTab="1"/>
+    <workbookView windowWidth="20490" windowHeight="7980" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Default" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Employee ID</t>
   </si>
@@ -59,10 +59,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -79,9 +79,38 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -100,98 +129,55 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -205,9 +191,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -222,14 +215,21 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -244,31 +244,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -280,73 +388,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -358,73 +424,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -453,26 +453,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -494,15 +494,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -515,166 +506,178 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
@@ -682,6 +685,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
   </cellXfs>
@@ -1005,55 +1009,55 @@
   <sheetPr/>
   <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.1428571428571" style="2" customWidth="1"/>
-    <col min="2" max="2" width="15.7142857142857" style="2" customWidth="1"/>
-    <col min="3" max="3" width="12.5714285714286" style="3" customWidth="1"/>
-    <col min="4" max="4" width="18" style="3" customWidth="1"/>
-    <col min="5" max="5" width="9.59047619047619" style="3" customWidth="1"/>
-    <col min="6" max="6" width="17.2857142857143" style="3" customWidth="1"/>
-    <col min="7" max="7" width="12.4190476190476" style="3" customWidth="1"/>
-    <col min="8" max="8" width="17.7142857142857" style="3" customWidth="1"/>
-    <col min="9" max="9" width="60.5904761904762" style="3" customWidth="1"/>
-    <col min="10" max="10" width="10.5809523809524" style="3" customWidth="1"/>
-    <col min="11" max="1025" width="8.66666666666667" style="3" customWidth="1"/>
-    <col min="1026" max="16384" width="9" style="3"/>
+    <col min="1" max="1" width="12.1428571428571" style="3" customWidth="1"/>
+    <col min="2" max="2" width="15.7142857142857" style="3" customWidth="1"/>
+    <col min="3" max="3" width="12.5714285714286" style="4" customWidth="1"/>
+    <col min="4" max="4" width="18" style="4" customWidth="1"/>
+    <col min="5" max="5" width="9.59047619047619" style="4" customWidth="1"/>
+    <col min="6" max="6" width="17.2857142857143" style="4" customWidth="1"/>
+    <col min="7" max="7" width="12.4190476190476" style="4" customWidth="1"/>
+    <col min="8" max="8" width="17.7142857142857" style="4" customWidth="1"/>
+    <col min="9" max="9" width="60.5904761904762" style="4" customWidth="1"/>
+    <col min="10" max="10" width="10.5809523809524" style="4" customWidth="1"/>
+    <col min="11" max="1025" width="8.66666666666667" style="5" customWidth="1"/>
+    <col min="1026" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="7" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1081,25 +1085,26 @@
   <sheetPr/>
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="18.2857142857143" customWidth="1"/>
+    <col min="1" max="1" width="22" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.2857142857143" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" selectLockedCells="1" objects="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
 </worksheet>

</xml_diff>